<commit_message>
Config table StptAdvancedAnalog done. Minor bug fix.
</commit_message>
<xml_diff>
--- a/Config Files/AdvancedAnalog_V0.xlsx
+++ b/Config Files/AdvancedAnalog_V0.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD11CCF1-165F-406E-BF07-1469CD61DFCC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB786094-0886-44C5-94EE-BA1E4973D296}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,259 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{2B1025A4-B7EC-4C4E-87D5-BFE96D196A94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ID iz tablice stringova u weinteku
+[008] SetpointsAdvancedAnalog</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{99D95F0F-798D-4EFC-9949-6C81DB121EF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+registar za provjeru postojanja stignala</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{F0900F9D-2B4D-4F16-A6E8-A84B4C6CAA24}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+adresa za provjeru postojanja adrese</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{94E20121-5AF8-46A5-B9BA-C2203D3B93A6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DW za provjeru postojanja signala</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{9BEC4E45-2126-4B23-837D-4EDBF40980E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+uvijet za provjeru postojanja signala</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{4E1531FE-F44A-4991-9D54-B5171604D6C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+pozicija bita u DW-u za provjeru postojanja signala</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{940CBBA3-5BD3-4171-BAC5-BA3006CF3E72}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+registar signala</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{1C7FA394-E51C-49A3-A209-B4B33982A48B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+adresa signala</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{9E7E5D7E-5B4E-43D8-852E-039549A58359}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+onemogućeno upisivanje vrijednosti</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{D00DBB64-4BD2-42D2-9970-E0D85F9F867C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+modbus data type</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t>Version: 1</t>
   </si>
@@ -68,13 +319,118 @@
   </si>
   <si>
     <t>High limit</t>
+  </si>
+  <si>
+    <t>Fire damper</t>
+  </si>
+  <si>
+    <t>VAV number</t>
+  </si>
+  <si>
+    <t>Scale supply air pressure</t>
+  </si>
+  <si>
+    <t>Scale extract air press</t>
+  </si>
+  <si>
+    <t>Build prot tmp deadz</t>
+  </si>
+  <si>
+    <t>VRF - dT1</t>
+  </si>
+  <si>
+    <t>VRF - dT2</t>
+  </si>
+  <si>
+    <t>Min-fact supply fan</t>
+  </si>
+  <si>
+    <t>Max-fact supply fan</t>
+  </si>
+  <si>
+    <t>Min-fact extract fan</t>
+  </si>
+  <si>
+    <t>Max-fact extract fan</t>
+  </si>
+  <si>
+    <t>Start up delay 1</t>
+  </si>
+  <si>
+    <t>Pre htg min offtime 1</t>
+  </si>
+  <si>
+    <t>Start up delay 2</t>
+  </si>
+  <si>
+    <t>Pre htg min offtime 2</t>
+  </si>
+  <si>
+    <t>Fire dmpr open time</t>
+  </si>
+  <si>
+    <t>0x2303 0x000088B4</t>
+  </si>
+  <si>
+    <t>0x2303 0x0000413A</t>
+  </si>
+  <si>
+    <t>0x2301 'InOutp\InOutp.ScaleSupplyPressure'</t>
+  </si>
+  <si>
+    <t>0x2301 'InOutp\InOutp.ScaleExhaustPressure'</t>
+  </si>
+  <si>
+    <t>0x2301 'Unit1\TempControl.DeadBandStdby'</t>
+  </si>
+  <si>
+    <t>0x2301 'Unit1\TempControl.VRF.dT_VRFbydT'</t>
+  </si>
+  <si>
+    <t>0x2301 'Unit1\TempControl.VRF.dT_VRFbydT2'</t>
+  </si>
+  <si>
+    <t>0x2301 'Unit1\FanControl.AirQMinFacSuFan'</t>
+  </si>
+  <si>
+    <t>0x2301 'Unit1\FanControl.AirQMaxFacSuFan'</t>
+  </si>
+  <si>
+    <t>&lt; 2</t>
+  </si>
+  <si>
+    <t>0x2301 'Unit1\FanControl.AirQMinFacExFan'</t>
+  </si>
+  <si>
+    <t>0x2301 'Unit1\FanControl.AirQMaxFacExFan'</t>
+  </si>
+  <si>
+    <t>0x2300 'Unit1\FanControlDelayOnWSel.DlyOnTm1'</t>
+  </si>
+  <si>
+    <t>&gt; 0</t>
+  </si>
+  <si>
+    <t>0x2300 'Unit1\FanControlDelayOnWSel.DlyOnTm2'</t>
+  </si>
+  <si>
+    <t>0x2300 'Unit1\FanControlDelayOnWSel1.DlyOnTm1'</t>
+  </si>
+  <si>
+    <t>0x2300 'Unit1\FanControlDelayOnWSel1.DlyOnTm2'</t>
+  </si>
+  <si>
+    <t>0x2300 'Unit1\DigitalInp.FDampInputs.FDampAlmTiDly'</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +446,24 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,14 +486,184 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC8C8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -394,21 +938,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -455,8 +1009,881 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>802</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>830</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>14</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>164</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>165</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>124</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0.1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>181</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0.1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9">
+        <v>17</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>182</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0.1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>805</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>111</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>50</v>
+      </c>
+      <c r="O10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>805</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>112</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>805</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>113</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>50</v>
+      </c>
+      <c r="O12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>805</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>114</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>100</v>
+      </c>
+      <c r="O13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>809</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>117</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>809</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>118</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>810</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>119</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>810</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>120</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>802</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>33</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="cellIs" dxfId="23" priority="24" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="21" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="cellIs" dxfId="19" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="17" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="15" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="14" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:A9">
+    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:A9">
+    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:A11">
+    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:A11">
+    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:A13">
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:A13">
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16:A17">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16:A17">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"To translate"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>